<commit_message>
Fixed Application Running Info
</commit_message>
<xml_diff>
--- a/examples/example-classroom_seating_plan-org.xlsx
+++ b/examples/example-classroom_seating_plan-org.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4809C8D3-DFF6-409F-8C43-48A2407A5785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3758AF9F-FBAD-481E-9687-FC152A99E8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Organised Zones</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>row_back_right</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -778,68 +781,74 @@
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -848,16 +857,22 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -894,86 +909,98 @@
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J3" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="F4" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Carring Certain Iterations and Added Disabling Dropping Iteration Count
</commit_message>
<xml_diff>
--- a/examples/example-classroom_seating_plan-org.xlsx
+++ b/examples/example-classroom_seating_plan-org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9928872C-1CF2-472F-B4FE-5F1F12704F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772AA5FC-A18B-4530-B423-3486F5B61096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -312,13 +312,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,30 +646,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
@@ -679,91 +679,91 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1"/>
@@ -784,55 +784,55 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,31 +840,31 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -872,25 +872,25 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -918,49 +918,49 @@
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,31 +968,31 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1000,25 +1000,25 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>

</xml_diff>